<commit_message>
all logic is expressed. Time to refactor. improve the code
</commit_message>
<xml_diff>
--- a/KeremetForms/Result/client_12345678901484.xlsx
+++ b/KeremetForms/Result/client_12345678901484.xlsx
@@ -63,10 +63,10 @@
     <t xml:space="preserve">Customer-250</t>
   </si>
   <si>
-    <t xml:space="preserve">586</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Нарын</t>
+    <t xml:space="preserve">261</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Бишкек</t>
   </si>
   <si>
     <t xml:space="preserve">12345678901484</t>
@@ -712,7 +712,7 @@
         <v>13</v>
       </c>
       <c r="F4" s="16">
-        <v>36447</v>
+        <v>35286</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>14</v>
@@ -746,7 +746,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="18">
-        <v>36447</v>
+        <v>35286</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>

</xml_diff>